<commit_message>
Refactor sake DB app: RBAC, meeting grouping, admin edit, audit log
</commit_message>
<xml_diff>
--- a/audit_log.xlsx
+++ b/audit_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45958.49250963149</v>
+        <v>45958.49250962963</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -550,6 +550,252 @@
         </is>
       </c>
       <c r="H3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45960.44648920139</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>145</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>テスト酒</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>{'id': 145, '会員氏名': 'テストくん', 'name': 'テスト酒', '蔵元': '', '地域': '', 'category': '', '精米歩合': '50', 'updated_at': Timestamp('2025-10-30 10:42:56.512101'), '備考': ''}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45960.58553192129</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>146</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>テスト２</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>{'id': 146, '会員氏名': 'テストくん', 'name': 'テスト２', '蔵元': '', '地域': '', 'category': '', '精米歩合': '', 'updated_at': Timestamp('2025-10-30 14:03:09.842204'), '備考': '', '例会': '登録承認待ち'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45960.58623380787</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>update_meeting</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>146</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>{'id': 146, '例会': '第24回'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45960.59161622685</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>update_meeting</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>145</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>テスト酒</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>例会</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>{'id': 145, 'name': 'テスト酒', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 10:42:56.512000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': '50', '備考': nan, '例会': nan, '例会日時': NaT}</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>{'id': 145, 'name': 'テスト酒', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 10:42:56.512000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': '50', '備考': nan, '例会': '24', '例会日時': NaT}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45960.5966872338</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>update_meeting</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>145</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>テスト酒</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>例会</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>{'id': 145, 'name': 'テスト酒', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 10:42:56.512000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': '50', '備考': nan, '例会': '24', '例会日時': NaT}</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>{'id': 145, 'name': 'テスト酒', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 10:42:56.512000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': '50', '備考': nan, '例会': '25', '例会日時': NaT}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45960.59791274305</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>update_meeting</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>146</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>テスト２</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>例会</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>{'id': 146, 'name': 'テスト２', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 14:03:09.842000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': nan, '備考': nan, '例会': '第24回', '例会日時': NaT}</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>{'id': 146, 'name': 'テスト２', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 14:03:09.842000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': nan, '備考': nan, '例会': '26', '例会日時': NaT}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45960.60267283207</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>delete</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>146</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>テスト２</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{'id': 146, 'name': 'テスト２', 'category': nan, 'quantity': nan, 'updated_at': Timestamp('2025-10-30 14:03:09.842000'), '会員氏名': 'テストくん', '蔵元': nan, '地域': nan, '精米歩合': nan, '備考': nan, '例会': 26, '例会日時': NaT}</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>{}</t>
         </is>

</xml_diff>